<commit_message>
se agrega el modulo 1 y 3 el 3 a medias por que faltan excel
</commit_message>
<xml_diff>
--- a/Parte1/Datos/precio_electricidad_vf.xlsx
+++ b/Parte1/Datos/precio_electricidad_vf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Desktop\ProyectoFondecyt\Parte1\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F614E77-97C5-47BC-A20D-904E2B9A558D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366E8ED6-B7B3-496A-B0FC-E492382046D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{16B8AABA-ABB8-4C54-AD91-D0DDDF0AF5E4}"/>
+    <workbookView xWindow="5265" yWindow="4185" windowWidth="11895" windowHeight="11295" xr2:uid="{16B8AABA-ABB8-4C54-AD91-D0DDDF0AF5E4}"/>
   </bookViews>
   <sheets>
     <sheet name="low" sheetId="1" r:id="rId1"/>
@@ -38,13 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="564">
-  <si>
-    <t>medium</t>
-  </si>
-  <si>
-    <t>high</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="566">
   <si>
     <t>periodo</t>
   </si>
@@ -1726,10 +1720,22 @@
     <t>0.1284</t>
   </si>
   <si>
-    <t>low1</t>
-  </si>
-  <si>
-    <t>low2</t>
+    <t>lowCLP</t>
+  </si>
+  <si>
+    <t>lowUSD</t>
+  </si>
+  <si>
+    <t>mediumCLP</t>
+  </si>
+  <si>
+    <t>mediumUSD</t>
+  </si>
+  <si>
+    <t>highCLP</t>
+  </si>
+  <si>
+    <t>highUSD</t>
   </si>
 </sst>
 </file>
@@ -2110,21 +2116,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{012787B3-CA59-458C-8985-C89394597BC1}">
   <dimension ref="A1:D326"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A305" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C1" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2132,10 +2138,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2143,10 +2149,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2157,7 +2163,7 @@
         <v>161</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2165,10 +2171,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2176,10 +2182,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2187,10 +2193,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2198,10 +2204,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2209,10 +2215,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2220,10 +2226,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2231,10 +2237,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2242,10 +2248,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2256,7 +2262,7 @@
         <v>159</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2264,10 +2270,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2275,10 +2281,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2286,10 +2292,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2297,10 +2303,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2308,10 +2314,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2319,10 +2325,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2333,7 +2339,7 @@
         <v>157437</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2341,10 +2347,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2355,7 +2361,7 @@
         <v>182</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2363,10 +2369,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2374,10 +2380,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2385,10 +2391,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2396,10 +2402,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2407,10 +2413,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2418,10 +2424,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2429,10 +2435,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2443,7 +2449,7 @@
         <v>254</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2451,10 +2457,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2462,10 +2468,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2473,10 +2479,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C33" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2484,10 +2490,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C34" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -2495,10 +2501,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C35" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -2509,7 +2515,7 @@
         <v>253</v>
       </c>
       <c r="C36" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -2517,10 +2523,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C37" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -2528,10 +2534,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C38" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -2539,10 +2545,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -2550,10 +2556,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C40" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -2561,10 +2567,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C41" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -2572,10 +2578,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C42" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -2583,10 +2589,10 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C43" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -2594,10 +2600,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C44" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -2605,10 +2611,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C45" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -2616,10 +2622,10 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C46" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -2627,10 +2633,10 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C47" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -2638,10 +2644,10 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C48" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -2649,10 +2655,10 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C49" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -2660,10 +2666,10 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C50" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -2671,10 +2677,10 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C51" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -2682,10 +2688,10 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C52" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -2693,10 +2699,10 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C53" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -2704,10 +2710,10 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C54" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -2715,10 +2721,10 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C55" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -2726,10 +2732,10 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C56" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -2737,10 +2743,10 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C57" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -2748,10 +2754,10 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C58" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -2759,10 +2765,10 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C59" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -2770,10 +2776,10 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C60" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -2781,10 +2787,10 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C61" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -2792,10 +2798,10 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C62" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -2803,10 +2809,10 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C63" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -2814,10 +2820,10 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C64" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -2825,10 +2831,10 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C65" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -2836,10 +2842,10 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C66" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -2847,10 +2853,10 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C67" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -2858,10 +2864,10 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C68" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -2869,10 +2875,10 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C69" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -2880,10 +2886,10 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C70" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -2894,7 +2900,7 @@
         <v>203</v>
       </c>
       <c r="C71" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -2902,10 +2908,10 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C72" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -2913,10 +2919,10 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C73" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -2924,10 +2930,10 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C74" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -2935,10 +2941,10 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C75" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -2946,10 +2952,10 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C76" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -2957,10 +2963,10 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C77" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -2968,10 +2974,10 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C78" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -2982,7 +2988,7 @@
         <v>193</v>
       </c>
       <c r="C79" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -2990,10 +2996,10 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C80" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -3001,10 +3007,10 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C81" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -3012,10 +3018,10 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C82" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -3023,10 +3029,10 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C83" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -3037,7 +3043,7 @@
         <v>187</v>
       </c>
       <c r="C84" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -3045,10 +3051,10 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C85" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -3056,10 +3062,10 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C86" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -3067,10 +3073,10 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C87" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -3078,10 +3084,10 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C88" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -3089,10 +3095,10 @@
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C89" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -3103,7 +3109,7 @@
         <v>180</v>
       </c>
       <c r="C90" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -3111,10 +3117,10 @@
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C91" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -3122,10 +3128,10 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C92" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -3133,10 +3139,10 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C93" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -3144,10 +3150,10 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C94" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -3155,10 +3161,10 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C95" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -3166,10 +3172,10 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C96" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -3177,10 +3183,10 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C97" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -3188,10 +3194,10 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C98" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -3199,10 +3205,10 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C99" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -3210,10 +3216,10 @@
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C100" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -3224,7 +3230,7 @@
         <v>168</v>
       </c>
       <c r="C101" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -3232,10 +3238,10 @@
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C102" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -3243,10 +3249,10 @@
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C103" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -3254,10 +3260,10 @@
         <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C104" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -3265,10 +3271,10 @@
         <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C105" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -3276,10 +3282,10 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C106" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -3287,10 +3293,10 @@
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C107" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -3298,10 +3304,10 @@
         <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C108" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -3309,10 +3315,10 @@
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C109" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -3320,10 +3326,10 @@
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C110" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -3331,10 +3337,10 @@
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C111" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -3342,10 +3348,10 @@
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C112" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -3353,10 +3359,10 @@
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C113" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -3364,10 +3370,10 @@
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C114" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -3375,10 +3381,10 @@
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C115" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -3386,10 +3392,10 @@
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C116" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -3397,10 +3403,10 @@
         <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C117" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -3408,10 +3414,10 @@
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C118" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -3422,7 +3428,7 @@
         <v>150</v>
       </c>
       <c r="C119" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -3433,7 +3439,7 @@
         <v>149</v>
       </c>
       <c r="C120" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -3441,10 +3447,10 @@
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C121" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -3452,10 +3458,10 @@
         <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C122" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -3463,10 +3469,10 @@
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C123" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -3474,10 +3480,10 @@
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C124" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -3485,10 +3491,10 @@
         <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C125" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -3496,10 +3502,10 @@
         <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C126" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -3507,10 +3513,10 @@
         <v>125</v>
       </c>
       <c r="B127" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C127" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -3518,10 +3524,10 @@
         <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C128" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -3529,10 +3535,10 @@
         <v>127</v>
       </c>
       <c r="B129" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C129" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -3540,10 +3546,10 @@
         <v>128</v>
       </c>
       <c r="B130" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C130" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -3554,7 +3560,7 @@
         <v>139</v>
       </c>
       <c r="C131" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -3562,10 +3568,10 @@
         <v>130</v>
       </c>
       <c r="B132" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C132" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -3573,10 +3579,10 @@
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C133" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -3584,10 +3590,10 @@
         <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C134" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -3595,10 +3601,10 @@
         <v>133</v>
       </c>
       <c r="B135" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C135" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D135" s="4"/>
     </row>
@@ -3607,10 +3613,10 @@
         <v>134</v>
       </c>
       <c r="B136" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C136" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -3618,10 +3624,10 @@
         <v>135</v>
       </c>
       <c r="B137" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C137" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -3632,7 +3638,7 @@
         <v>136</v>
       </c>
       <c r="C138" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -3640,10 +3646,10 @@
         <v>137</v>
       </c>
       <c r="B139" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C139" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -3651,10 +3657,10 @@
         <v>138</v>
       </c>
       <c r="B140" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C140" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -3662,10 +3668,10 @@
         <v>139</v>
       </c>
       <c r="B141" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C141" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -3673,10 +3679,10 @@
         <v>140</v>
       </c>
       <c r="B142" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C142" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -3684,10 +3690,10 @@
         <v>141</v>
       </c>
       <c r="B143" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C143" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -3695,10 +3701,10 @@
         <v>142</v>
       </c>
       <c r="B144" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C144" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -3706,10 +3712,10 @@
         <v>143</v>
       </c>
       <c r="B145" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C145" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -3717,10 +3723,10 @@
         <v>144</v>
       </c>
       <c r="B146" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C146" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -3728,10 +3734,10 @@
         <v>145</v>
       </c>
       <c r="B147" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C147" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -3739,10 +3745,10 @@
         <v>146</v>
       </c>
       <c r="B148" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C148" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -3753,7 +3759,7 @@
         <v>135</v>
       </c>
       <c r="C149" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -3761,10 +3767,10 @@
         <v>148</v>
       </c>
       <c r="B150" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C150" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -3772,10 +3778,10 @@
         <v>149</v>
       </c>
       <c r="B151" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C151" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -3783,10 +3789,10 @@
         <v>150</v>
       </c>
       <c r="B152" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C152" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -3794,10 +3800,10 @@
         <v>151</v>
       </c>
       <c r="B153" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C153" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -3805,10 +3811,10 @@
         <v>152</v>
       </c>
       <c r="B154" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C154" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -3816,10 +3822,10 @@
         <v>153</v>
       </c>
       <c r="B155" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C155" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -3827,10 +3833,10 @@
         <v>154</v>
       </c>
       <c r="B156" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C156" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -3838,10 +3844,10 @@
         <v>155</v>
       </c>
       <c r="B157" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C157" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -3849,10 +3855,10 @@
         <v>156</v>
       </c>
       <c r="B158" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C158" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -3860,10 +3866,10 @@
         <v>157</v>
       </c>
       <c r="B159" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C159" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -3874,7 +3880,7 @@
         <v>134</v>
       </c>
       <c r="C160" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -3885,7 +3891,7 @@
         <v>134</v>
       </c>
       <c r="C161" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -3893,10 +3899,10 @@
         <v>160</v>
       </c>
       <c r="B162" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C162" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -3904,10 +3910,10 @@
         <v>161</v>
       </c>
       <c r="B163" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C163" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -3915,10 +3921,10 @@
         <v>162</v>
       </c>
       <c r="B164" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C164" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -3926,10 +3932,10 @@
         <v>163</v>
       </c>
       <c r="B165" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C165" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -3937,10 +3943,10 @@
         <v>164</v>
       </c>
       <c r="B166" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C166" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -3948,10 +3954,10 @@
         <v>165</v>
       </c>
       <c r="B167" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C167" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -3959,10 +3965,10 @@
         <v>166</v>
       </c>
       <c r="B168" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C168" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -3970,10 +3976,10 @@
         <v>167</v>
       </c>
       <c r="B169" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C169" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -3981,10 +3987,10 @@
         <v>168</v>
       </c>
       <c r="B170" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C170" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -3992,10 +3998,10 @@
         <v>169</v>
       </c>
       <c r="B171" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C171" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -4006,7 +4012,7 @@
         <v>133</v>
       </c>
       <c r="C172" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -4014,10 +4020,10 @@
         <v>171</v>
       </c>
       <c r="B173" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C173" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -4025,10 +4031,10 @@
         <v>172</v>
       </c>
       <c r="B174" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C174" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -4036,10 +4042,10 @@
         <v>173</v>
       </c>
       <c r="B175" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C175" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -4047,10 +4053,10 @@
         <v>174</v>
       </c>
       <c r="B176" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C176" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -4058,10 +4064,10 @@
         <v>175</v>
       </c>
       <c r="B177" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C177" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -4069,10 +4075,10 @@
         <v>176</v>
       </c>
       <c r="B178" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C178" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -4080,10 +4086,10 @@
         <v>177</v>
       </c>
       <c r="B179" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C179" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -4091,10 +4097,10 @@
         <v>178</v>
       </c>
       <c r="B180" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C180" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -4102,10 +4108,10 @@
         <v>179</v>
       </c>
       <c r="B181" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C181" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -4113,10 +4119,10 @@
         <v>180</v>
       </c>
       <c r="B182" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C182" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -4127,7 +4133,7 @@
         <v>132</v>
       </c>
       <c r="C183" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -4135,10 +4141,10 @@
         <v>182</v>
       </c>
       <c r="B184" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C184" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
@@ -4146,10 +4152,10 @@
         <v>183</v>
       </c>
       <c r="B185" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C185" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
@@ -4157,10 +4163,10 @@
         <v>184</v>
       </c>
       <c r="B186" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C186" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
@@ -4168,10 +4174,10 @@
         <v>185</v>
       </c>
       <c r="B187" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C187" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -4179,10 +4185,10 @@
         <v>186</v>
       </c>
       <c r="B188" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C188" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
@@ -4190,10 +4196,10 @@
         <v>187</v>
       </c>
       <c r="B189" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C189" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
@@ -4201,10 +4207,10 @@
         <v>188</v>
       </c>
       <c r="B190" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C190" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
@@ -4212,10 +4218,10 @@
         <v>189</v>
       </c>
       <c r="B191" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C191" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
@@ -4223,10 +4229,10 @@
         <v>190</v>
       </c>
       <c r="B192" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C192" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
@@ -4234,10 +4240,10 @@
         <v>191</v>
       </c>
       <c r="B193" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C193" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -4248,7 +4254,7 @@
         <v>131</v>
       </c>
       <c r="C194" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -4256,10 +4262,10 @@
         <v>193</v>
       </c>
       <c r="B195" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C195" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -4267,10 +4273,10 @@
         <v>194</v>
       </c>
       <c r="B196" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C196" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -4278,10 +4284,10 @@
         <v>195</v>
       </c>
       <c r="B197" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C197" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -4289,10 +4295,10 @@
         <v>196</v>
       </c>
       <c r="B198" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C198" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -4300,10 +4306,10 @@
         <v>197</v>
       </c>
       <c r="B199" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C199" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -4311,10 +4317,10 @@
         <v>198</v>
       </c>
       <c r="B200" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C200" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -4322,10 +4328,10 @@
         <v>199</v>
       </c>
       <c r="B201" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C201" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
@@ -4333,10 +4339,10 @@
         <v>200</v>
       </c>
       <c r="B202" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C202" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
@@ -4344,10 +4350,10 @@
         <v>201</v>
       </c>
       <c r="B203" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C203" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
@@ -4355,10 +4361,10 @@
         <v>202</v>
       </c>
       <c r="B204" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C204" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
@@ -4366,10 +4372,10 @@
         <v>203</v>
       </c>
       <c r="B205" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C205" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
@@ -4380,7 +4386,7 @@
         <v>130</v>
       </c>
       <c r="C206" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
@@ -4388,10 +4394,10 @@
         <v>205</v>
       </c>
       <c r="B207" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C207" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
@@ -4399,10 +4405,10 @@
         <v>206</v>
       </c>
       <c r="B208" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C208" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
@@ -4410,10 +4416,10 @@
         <v>207</v>
       </c>
       <c r="B209" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C209" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
@@ -4421,10 +4427,10 @@
         <v>208</v>
       </c>
       <c r="B210" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C210" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
@@ -4432,10 +4438,10 @@
         <v>209</v>
       </c>
       <c r="B211" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C211" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
@@ -4443,10 +4449,10 @@
         <v>210</v>
       </c>
       <c r="B212" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C212" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
@@ -4454,10 +4460,10 @@
         <v>211</v>
       </c>
       <c r="B213" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C213" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
@@ -4465,10 +4471,10 @@
         <v>212</v>
       </c>
       <c r="B214" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C214" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
@@ -4476,10 +4482,10 @@
         <v>213</v>
       </c>
       <c r="B215" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C215" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
@@ -4487,10 +4493,10 @@
         <v>214</v>
       </c>
       <c r="B216" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C216" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
@@ -4501,7 +4507,7 @@
         <v>129</v>
       </c>
       <c r="C217" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
@@ -4509,10 +4515,10 @@
         <v>216</v>
       </c>
       <c r="B218" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C218" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
@@ -4520,10 +4526,10 @@
         <v>217</v>
       </c>
       <c r="B219" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C219" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
@@ -4531,10 +4537,10 @@
         <v>218</v>
       </c>
       <c r="B220" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C220" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
@@ -4542,10 +4548,10 @@
         <v>219</v>
       </c>
       <c r="B221" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C221" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
@@ -4553,10 +4559,10 @@
         <v>220</v>
       </c>
       <c r="B222" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C222" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
@@ -4564,10 +4570,10 @@
         <v>221</v>
       </c>
       <c r="B223" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C223" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
@@ -4575,10 +4581,10 @@
         <v>222</v>
       </c>
       <c r="B224" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C224" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -4586,10 +4592,10 @@
         <v>223</v>
       </c>
       <c r="B225" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C225" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
@@ -4597,10 +4603,10 @@
         <v>224</v>
       </c>
       <c r="B226" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C226" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
@@ -4608,10 +4614,10 @@
         <v>225</v>
       </c>
       <c r="B227" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C227" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
@@ -4619,10 +4625,10 @@
         <v>226</v>
       </c>
       <c r="B228" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C228" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
@@ -4633,7 +4639,7 @@
         <v>128</v>
       </c>
       <c r="C229" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
@@ -4641,10 +4647,10 @@
         <v>228</v>
       </c>
       <c r="B230" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C230" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
@@ -4652,10 +4658,10 @@
         <v>229</v>
       </c>
       <c r="B231" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C231" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
@@ -4663,10 +4669,10 @@
         <v>230</v>
       </c>
       <c r="B232" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C232" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
@@ -4674,10 +4680,10 @@
         <v>231</v>
       </c>
       <c r="B233" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C233" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
@@ -4685,10 +4691,10 @@
         <v>232</v>
       </c>
       <c r="B234" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C234" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
@@ -4696,10 +4702,10 @@
         <v>233</v>
       </c>
       <c r="B235" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C235" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
@@ -4707,10 +4713,10 @@
         <v>234</v>
       </c>
       <c r="B236" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C236" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
@@ -4718,10 +4724,10 @@
         <v>235</v>
       </c>
       <c r="B237" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C237" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
@@ -4729,10 +4735,10 @@
         <v>236</v>
       </c>
       <c r="B238" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C238" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
@@ -4740,10 +4746,10 @@
         <v>237</v>
       </c>
       <c r="B239" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C239" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
@@ -4751,10 +4757,10 @@
         <v>238</v>
       </c>
       <c r="B240" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C240" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
@@ -4765,7 +4771,7 @@
         <v>127</v>
       </c>
       <c r="C241" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
@@ -4773,10 +4779,10 @@
         <v>240</v>
       </c>
       <c r="B242" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C242" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
@@ -4784,10 +4790,10 @@
         <v>241</v>
       </c>
       <c r="B243" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C243" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
@@ -4795,10 +4801,10 @@
         <v>242</v>
       </c>
       <c r="B244" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C244" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
@@ -4806,10 +4812,10 @@
         <v>243</v>
       </c>
       <c r="B245" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C245" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
@@ -4817,10 +4823,10 @@
         <v>244</v>
       </c>
       <c r="B246" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C246" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
@@ -4828,10 +4834,10 @@
         <v>245</v>
       </c>
       <c r="B247" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C247" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
@@ -4839,10 +4845,10 @@
         <v>246</v>
       </c>
       <c r="B248" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C248" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
@@ -4850,10 +4856,10 @@
         <v>247</v>
       </c>
       <c r="B249" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C249" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
@@ -4861,10 +4867,10 @@
         <v>248</v>
       </c>
       <c r="B250" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C250" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
@@ -4872,10 +4878,10 @@
         <v>249</v>
       </c>
       <c r="B251" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C251" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
@@ -4886,7 +4892,7 @@
         <v>126</v>
       </c>
       <c r="C252" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
@@ -4897,7 +4903,7 @@
         <v>126</v>
       </c>
       <c r="C253" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
@@ -4905,10 +4911,10 @@
         <v>252</v>
       </c>
       <c r="B254" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C254" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
@@ -4916,10 +4922,10 @@
         <v>253</v>
       </c>
       <c r="B255" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C255" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
@@ -4927,10 +4933,10 @@
         <v>254</v>
       </c>
       <c r="B256" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C256" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
@@ -4938,10 +4944,10 @@
         <v>255</v>
       </c>
       <c r="B257" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C257" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
@@ -4949,10 +4955,10 @@
         <v>256</v>
       </c>
       <c r="B258" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C258" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
@@ -4960,10 +4966,10 @@
         <v>257</v>
       </c>
       <c r="B259" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C259" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
@@ -4971,10 +4977,10 @@
         <v>258</v>
       </c>
       <c r="B260" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C260" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
@@ -4982,10 +4988,10 @@
         <v>259</v>
       </c>
       <c r="B261" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C261" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
@@ -4993,10 +4999,10 @@
         <v>260</v>
       </c>
       <c r="B262" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C262" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
@@ -5004,10 +5010,10 @@
         <v>261</v>
       </c>
       <c r="B263" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C263" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
@@ -5018,7 +5024,7 @@
         <v>125</v>
       </c>
       <c r="C264" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
@@ -5029,7 +5035,7 @@
         <v>125</v>
       </c>
       <c r="C265" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
@@ -5037,10 +5043,10 @@
         <v>264</v>
       </c>
       <c r="B266" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C266" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
@@ -5048,10 +5054,10 @@
         <v>265</v>
       </c>
       <c r="B267" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C267" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
@@ -5059,10 +5065,10 @@
         <v>266</v>
       </c>
       <c r="B268" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C268" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
@@ -5070,10 +5076,10 @@
         <v>267</v>
       </c>
       <c r="B269" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C269" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
@@ -5081,10 +5087,10 @@
         <v>268</v>
       </c>
       <c r="B270" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C270" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
@@ -5092,10 +5098,10 @@
         <v>269</v>
       </c>
       <c r="B271" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C271" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
@@ -5103,10 +5109,10 @@
         <v>270</v>
       </c>
       <c r="B272" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C272" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
@@ -5114,10 +5120,10 @@
         <v>271</v>
       </c>
       <c r="B273" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C273" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
@@ -5125,10 +5131,10 @@
         <v>272</v>
       </c>
       <c r="B274" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C274" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
@@ -5136,10 +5142,10 @@
         <v>273</v>
       </c>
       <c r="B275" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C275" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
@@ -5150,7 +5156,7 @@
         <v>124</v>
       </c>
       <c r="C276" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
@@ -5161,7 +5167,7 @@
         <v>124</v>
       </c>
       <c r="C277" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
@@ -5169,10 +5175,10 @@
         <v>276</v>
       </c>
       <c r="B278" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C278" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
@@ -5180,10 +5186,10 @@
         <v>277</v>
       </c>
       <c r="B279" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C279" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
@@ -5191,10 +5197,10 @@
         <v>278</v>
       </c>
       <c r="B280" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C280" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
@@ -5202,10 +5208,10 @@
         <v>279</v>
       </c>
       <c r="B281" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C281" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
@@ -5213,10 +5219,10 @@
         <v>280</v>
       </c>
       <c r="B282" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C282" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
@@ -5224,10 +5230,10 @@
         <v>281</v>
       </c>
       <c r="B283" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C283" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
@@ -5235,10 +5241,10 @@
         <v>282</v>
       </c>
       <c r="B284" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C284" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
@@ -5246,10 +5252,10 @@
         <v>283</v>
       </c>
       <c r="B285" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C285" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
@@ -5257,10 +5263,10 @@
         <v>284</v>
       </c>
       <c r="B286" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C286" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
@@ -5268,10 +5274,10 @@
         <v>285</v>
       </c>
       <c r="B287" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C287" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
@@ -5282,7 +5288,7 @@
         <v>123</v>
       </c>
       <c r="C288" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
@@ -5293,7 +5299,7 @@
         <v>123</v>
       </c>
       <c r="C289" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
@@ -5301,10 +5307,10 @@
         <v>288</v>
       </c>
       <c r="B290" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C290" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
@@ -5312,10 +5318,10 @@
         <v>289</v>
       </c>
       <c r="B291" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C291" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
@@ -5323,10 +5329,10 @@
         <v>290</v>
       </c>
       <c r="B292" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C292" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
@@ -5334,10 +5340,10 @@
         <v>291</v>
       </c>
       <c r="B293" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C293" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
@@ -5345,10 +5351,10 @@
         <v>292</v>
       </c>
       <c r="B294" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C294" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
@@ -5356,10 +5362,10 @@
         <v>293</v>
       </c>
       <c r="B295" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C295" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
@@ -5367,10 +5373,10 @@
         <v>294</v>
       </c>
       <c r="B296" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C296" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
@@ -5378,10 +5384,10 @@
         <v>295</v>
       </c>
       <c r="B297" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C297" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
@@ -5389,10 +5395,10 @@
         <v>296</v>
       </c>
       <c r="B298" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C298" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
@@ -5400,10 +5406,10 @@
         <v>297</v>
       </c>
       <c r="B299" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C299" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
@@ -5411,10 +5417,10 @@
         <v>298</v>
       </c>
       <c r="B300" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C300" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
@@ -5425,7 +5431,7 @@
         <v>122</v>
       </c>
       <c r="C301" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
@@ -5433,10 +5439,10 @@
         <v>300</v>
       </c>
       <c r="B302" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C302" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
@@ -5444,10 +5450,10 @@
         <v>301</v>
       </c>
       <c r="B303" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C303" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
@@ -5455,10 +5461,10 @@
         <v>302</v>
       </c>
       <c r="B304" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C304" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
@@ -5466,10 +5472,10 @@
         <v>303</v>
       </c>
       <c r="B305" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C305" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
@@ -5477,10 +5483,10 @@
         <v>304</v>
       </c>
       <c r="B306" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C306" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
@@ -5488,10 +5494,10 @@
         <v>305</v>
       </c>
       <c r="B307" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C307" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
@@ -5499,10 +5505,10 @@
         <v>306</v>
       </c>
       <c r="B308" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C308" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
@@ -5510,10 +5516,10 @@
         <v>307</v>
       </c>
       <c r="B309" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C309" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
@@ -5521,10 +5527,10 @@
         <v>308</v>
       </c>
       <c r="B310" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C310" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
@@ -5532,10 +5538,10 @@
         <v>309</v>
       </c>
       <c r="B311" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C311" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
@@ -5543,10 +5549,10 @@
         <v>310</v>
       </c>
       <c r="B312" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C312" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
@@ -5557,7 +5563,7 @@
         <v>121</v>
       </c>
       <c r="C313" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
@@ -5565,10 +5571,10 @@
         <v>312</v>
       </c>
       <c r="B314" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C314" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
@@ -5576,10 +5582,10 @@
         <v>313</v>
       </c>
       <c r="B315" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C315" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
@@ -5587,10 +5593,10 @@
         <v>314</v>
       </c>
       <c r="B316" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C316" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
@@ -5598,10 +5604,10 @@
         <v>315</v>
       </c>
       <c r="B317" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C317" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
@@ -5609,10 +5615,10 @@
         <v>316</v>
       </c>
       <c r="B318" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C318" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
@@ -5620,10 +5626,10 @@
         <v>317</v>
       </c>
       <c r="B319" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C319" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
@@ -5631,10 +5637,10 @@
         <v>318</v>
       </c>
       <c r="B320" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C320" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
@@ -5642,10 +5648,10 @@
         <v>319</v>
       </c>
       <c r="B321" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C321" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.25">
@@ -5653,10 +5659,10 @@
         <v>320</v>
       </c>
       <c r="B322" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C322" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.25">
@@ -5664,10 +5670,10 @@
         <v>321</v>
       </c>
       <c r="B323" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C323" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
@@ -5675,10 +5681,10 @@
         <v>322</v>
       </c>
       <c r="B324" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C324" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
@@ -5689,7 +5695,7 @@
         <v>120</v>
       </c>
       <c r="C325" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">
@@ -5700,7 +5706,7 @@
         <v>120</v>
       </c>
       <c r="C326" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
   </sheetData>
@@ -5712,21 +5718,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CA0A2AF-54A2-47DE-A9D4-CB39189EED62}">
   <dimension ref="A1:C326"/>
   <sheetViews>
-    <sheetView topLeftCell="A287" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:J7"/>
+    <sheetView topLeftCell="A305" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>562</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>563</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -9313,21 +9319,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F83D9E1-D158-47CB-8FA7-14DACBFDC7BF}">
   <dimension ref="A1:F326"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A305" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>564</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>565</v>
       </c>
       <c r="F1" s="1"/>
     </row>

</xml_diff>